<commit_message>
IMU board V2 release candidate
</commit_message>
<xml_diff>
--- a/KiCAD/imu-board/BOM_for_PCBway.xlsx
+++ b/KiCAD/imu-board/BOM_for_PCBway.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t xml:space="preserve">NinjaNIRS IMU V2.0 Bill of Materials
 For Boston University</t>
@@ -165,9 +165,6 @@
     <t xml:space="preserve">LED RED CLEAR CHIP SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
     <t xml:space="preserve">J2</t>
   </si>
   <si>
@@ -229,6 +226,24 @@
   </si>
   <si>
     <t xml:space="preserve">28-VQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC065-06-A-L-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6POS 1.0MM PITCH SOCKET, SIL, TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-SIL 1MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THD</t>
   </si>
   <si>
     <t xml:space="preserve">Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!</t>
@@ -385,7 +400,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,23 +442,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -550,9 +549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>666360</xdr:colOff>
+      <xdr:colOff>666000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -566,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="209520"/>
-          <a:ext cx="1360080" cy="375840"/>
+          <a:ext cx="1359720" cy="375480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,7 +588,7 @@
   <dimension ref="A2:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -599,7 +598,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.63"/>
@@ -683,23 +682,23 @@
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -708,35 +707,35 @@
       <c r="H8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,19 +743,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>14</v>
@@ -771,22 +770,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>15</v>
@@ -798,66 +797,92 @@
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="E13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" s="19" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-    </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" s="15" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -870,12 +895,12 @@
   <mergeCells count="4">
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="D2:F4"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A18:I18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!"/>
-    <hyperlink ref="A17" r:id="rId2" display="Click for Instructions on How to Create a BOM"/>
+    <hyperlink ref="A16" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!"/>
+    <hyperlink ref="A18" r:id="rId2" display="Click for Instructions on How to Create a BOM"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -899,7 +924,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -922,7 +947,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>